<commit_message>
Rename file and Adding new Data
</commit_message>
<xml_diff>
--- a/04-10-2019-11.12.xlsx
+++ b/04-10-2019-11.12.xlsx
@@ -56,32 +56,27 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="5">
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
+  <fonts count="4">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="0"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="0"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="0"/>
     </font>
   </fonts>
   <fills count="2">
@@ -131,7 +126,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -155,12 +150,12 @@
   <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B6" activeCellId="0" sqref="B6"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="39.45"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="39.44"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="29.18"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="30.84"/>
   </cols>

</xml_diff>